<commit_message>
Proxy Aware test setup code added.
</commit_message>
<xml_diff>
--- a/West.EnterpriseUX.Automation/West.EnterpriseUX.Automation.MobileNew/TestData/DEV/LoginData.xlsx
+++ b/West.EnterpriseUX.Automation/West.EnterpriseUX.Automation.MobileNew/TestData/DEV/LoginData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patilg\source\repos\UAT_Test\EnterpriseUX.MobileAutomation\West.EnterpriseUX.Automation\West.EnterpriseUX.Automation.MobileNew\TestData\DVV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patilg\source\repos\UAT_Test\EnterpriseUX.MobileAutomation\West.EnterpriseUX.Automation\West.EnterpriseUX.Automation.MobileNew\TestData\DEV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3045B046-4DD3-4A63-9573-498AAF89DA1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2AF27E-A9A8-4C84-94D0-590BC2701E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1820" yWindow="1820" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
@@ -367,9 +367,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>